<commit_message>
few new negative tests; change to the way negative testing is done
</commit_message>
<xml_diff>
--- a/tests/shouldFail/undefined.xlsx
+++ b/tests/shouldFail/undefined.xlsx
@@ -1462,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,7 +1646,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -1657,7 +1657,7 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -2384,7 +2384,7 @@
       </c>
       <c r="B84">
         <f>SUM(B1:B82)</f>
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -2393,7 +2393,7 @@
       </c>
       <c r="B85">
         <f>B84/82</f>
-        <v>0.51219512195121952</v>
+        <v>0.53658536585365857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>